<commit_message>
Delete repeat description in two Beaufort categories
</commit_message>
<xml_diff>
--- a/data/Beaufort Wind Cats.xlsx
+++ b/data/Beaufort Wind Cats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francesleduke/Downloads/freelandbunker/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francesleduke/Downloads/freelandbunker copy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3F61D5-7C32-B24F-AF17-B7FD3882057B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E122AE99-BB15-4B41-B018-4C09864DA6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="940" windowWidth="25040" windowHeight="13680" xr2:uid="{E5CE1841-4437-5843-8766-FFFD97D03E47}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
   <si>
     <t xml:space="preserve">calm </t>
   </si>
@@ -251,9 +251,6 @@
   </si>
   <si>
     <t>squalls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hauled down </t>
   </si>
   <si>
     <t>blowing hard</t>
@@ -730,7 +727,7 @@
   <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,43 +748,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -822,7 +819,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>10</v>
@@ -1007,7 +1004,7 @@
         <v>65</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1051,49 +1048,49 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G17" s="1" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G18" s="1" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G19" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.2">
@@ -1103,12 +1100,12 @@
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G21" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G22" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="7:7" x14ac:dyDescent="0.2">
@@ -1126,10 +1123,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G26" s="1" t="s">
-        <v>86</v>
-      </c>
+    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G96" s="2"/>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
@@ -1213,13 +1208,15 @@
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
-      <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G103" s="2"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
@@ -1273,13 +1270,15 @@
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
-      <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G108" s="2"/>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
@@ -1363,7 +1362,6 @@
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
-      <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>

</xml_diff>

<commit_message>
Update Beaufort Cats xlsx
Remove "hauled" and "hauling" "hauling out" but keeping "hauling little" for now
</commit_message>
<xml_diff>
--- a/data/Beaufort Wind Cats.xlsx
+++ b/data/Beaufort Wind Cats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francesleduke/Downloads/freelandbunker copy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E122AE99-BB15-4B41-B018-4C09864DA6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C05B797-918B-F54D-88E9-8F083B1FB3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="940" windowWidth="25040" windowHeight="13680" xr2:uid="{E5CE1841-4437-5843-8766-FFFD97D03E47}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="98">
   <si>
     <t xml:space="preserve">calm </t>
   </si>
@@ -283,16 +283,7 @@
     <t>heavy breeze</t>
   </si>
   <si>
-    <t xml:space="preserve">hauled  </t>
-  </si>
-  <si>
-    <t>hauling</t>
-  </si>
-  <si>
     <t xml:space="preserve">blew very heavy </t>
-  </si>
-  <si>
-    <t>hauling out</t>
   </si>
   <si>
     <t>zero_knots</t>
@@ -727,7 +718,7 @@
   <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,7 +731,8 @@
     <col min="6" max="6" width="17.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="10" width="11" style="1"/>
+    <col min="9" max="9" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1"/>
     <col min="11" max="11" width="17" style="1" customWidth="1"/>
     <col min="12" max="12" width="14.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" style="1" customWidth="1"/>
@@ -748,43 +740,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -819,7 +811,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>10</v>
@@ -1004,7 +996,7 @@
         <v>65</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1039,6 +1031,9 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>70</v>
       </c>
@@ -1108,20 +1103,11 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G23" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G24" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G25" s="1" t="s">
-        <v>85</v>
-      </c>
+    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G95" s="2"/>
     </row>
     <row r="96" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G96" s="2"/>
@@ -1178,7 +1164,6 @@
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
@@ -1208,6 +1193,7 @@
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
@@ -1240,7 +1226,6 @@
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
-      <c r="G105" s="2"/>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
@@ -1270,6 +1255,7 @@
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
@@ -1332,7 +1318,6 @@
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
@@ -1347,7 +1332,6 @@
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
-      <c r="G113" s="2"/>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>

</xml_diff>